<commit_message>
Recover randk model size
</commit_message>
<xml_diff>
--- a/additional_experiments/cifar_dirichlet_server8/results.xlsx
+++ b/additional_experiments/cifar_dirichlet_server8/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Documents\GitHub\FLSim\additional_experiments\cifar_dirichlet_server8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41F42CB-B13F-4FB3-A5D7-AB6E5B0DBCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE2882D-3AA2-406E-BB8A-6CF4ACB853F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F0480BD0-FD3B-47B3-8709-724D203C8353}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="30">
   <si>
     <t>server qsgd bits</t>
   </si>
@@ -1244,13 +1244,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>207.53933333333336</c:v>
+                  <c:v>64.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>111.53093333333332</c:v>
+                  <c:v>67.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.562066666666681</c:v>
+                  <c:v>98.166666666666671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1309,13 +1309,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>167.75200000000001</c:v>
+                  <c:v>55.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>126.7146</c:v>
+                  <c:v>76.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.08873333333332</c:v>
+                  <c:v>114.83333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,13 +1440,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>758.25600000000009</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>758.25600000000009</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>758.25600000000009</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1766,35 +1766,43 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$41:$R$43</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$R$41:$R$43</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$R$41:$R$42</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>8-bit qsgd client</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4-bit qsgd client</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2-bit qsgd client</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$35:$T$37</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$T$35:$T$37</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$T$35:$T$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>207.53933333333336</c:v>
+                  <c:v>64.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>167.75200000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>55.666666666666664</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1838,35 +1846,43 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$41:$R$43</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$R$41:$R$43</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$R$41:$R$42</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>8-bit qsgd client</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4-bit qsgd client</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2-bit qsgd client</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$38:$T$40</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$T$38:$T$40</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$T$38:$T$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>111.53093333333332</c:v>
+                  <c:v>67.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>126.7146</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>76.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1903,35 +1919,43 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$41:$R$43</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$R$41:$R$43</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$R$41:$R$42</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>8-bit qsgd client</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4-bit qsgd client</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2-bit qsgd client</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$41:$T$43</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$T$41:$T$43</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$T$41:$T$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>85.562066666666681</c:v>
+                  <c:v>98.166666666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.08873333333332</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>114.83333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1984,20 +2008,40 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>8-bit qsgd client</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>4-bit qsgd client</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$35:$U$37</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$U$35:$U$37</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$U$35:$U$36</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>758.25600000000009</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>758.25600000000009</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>758.25600000000009</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2109,7 +2153,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>MB Broadcasted</a:t>
+                  <a:t>Client uploads (thousands)</a:t>
                 </a:r>
               </a:p>
               <a:p>
@@ -2333,13 +2377,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>207.53933333333336</c:v>
+                  <c:v>64.333333333333343</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>111.53093333333332</c:v>
+                  <c:v>67.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.562066666666681</c:v>
+                  <c:v>98.166666666666671</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2405,13 +2449,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>167.75200000000001</c:v>
+                  <c:v>55.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>126.7146</c:v>
+                  <c:v>76.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100.08873333333332</c:v>
+                  <c:v>114.83333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2536,13 +2580,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>758.25600000000009</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>758.25600000000009</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>758.25600000000009</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6004,8 +6048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A108EE6-3E1B-4A89-A28E-C5695062FD69}">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L18" workbookViewId="0">
-      <selection activeCell="V33" sqref="V33"/>
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="W39" sqref="W39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6712,6 +6756,9 @@
       <c r="O13" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="P13" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -6752,6 +6799,10 @@
         <f>N14/10</f>
         <v>758.25600000000009</v>
       </c>
+      <c r="P14" s="1">
+        <f>K14/1000</f>
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
@@ -6827,12 +6878,12 @@
         <v>10</v>
       </c>
       <c r="T19" s="1">
-        <f>T2</f>
-        <v>207.53933333333336</v>
+        <f>U2</f>
+        <v>64.333333333333343</v>
       </c>
       <c r="U19" s="1">
-        <f>$O$14</f>
-        <v>758.25600000000009</v>
+        <f>$P$14</f>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -6872,12 +6923,12 @@
         <v>11</v>
       </c>
       <c r="T20" s="1">
-        <f t="shared" ref="T20:T27" si="17">T3</f>
-        <v>111.53093333333332</v>
+        <f t="shared" ref="T20:T27" si="17">U3</f>
+        <v>67.333333333333329</v>
       </c>
       <c r="U20" s="1">
-        <f t="shared" ref="U20:U27" si="18">$O$14</f>
-        <v>758.25600000000009</v>
+        <f t="shared" ref="U20:U27" si="18">$P$14</f>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -6916,11 +6967,11 @@
       </c>
       <c r="T21" s="1">
         <f t="shared" si="17"/>
-        <v>85.562066666666681</v>
+        <v>98.166666666666671</v>
       </c>
       <c r="U21" s="1">
         <f t="shared" si="18"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -6956,11 +7007,11 @@
       </c>
       <c r="T22" s="1">
         <f t="shared" si="17"/>
-        <v>167.75200000000001</v>
+        <v>55.666666666666664</v>
       </c>
       <c r="U22" s="1">
         <f t="shared" si="18"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -6999,11 +7050,11 @@
       </c>
       <c r="T23" s="1">
         <f t="shared" si="17"/>
-        <v>126.7146</v>
+        <v>76.5</v>
       </c>
       <c r="U23" s="1">
         <f t="shared" si="18"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -7042,11 +7093,11 @@
       </c>
       <c r="T24" s="1">
         <f t="shared" si="17"/>
-        <v>100.08873333333332</v>
+        <v>114.83333333333333</v>
       </c>
       <c r="U24" s="1">
         <f t="shared" si="18"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -7086,7 +7137,7 @@
       </c>
       <c r="U25" s="1">
         <f t="shared" si="18"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -7129,7 +7180,7 @@
       </c>
       <c r="U26" s="1">
         <f t="shared" si="18"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -7172,7 +7223,7 @@
       </c>
       <c r="U27" s="1">
         <f t="shared" si="18"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
@@ -7223,11 +7274,11 @@
       </c>
       <c r="T35" s="1">
         <f>T49</f>
-        <v>207.53933333333336</v>
+        <v>64.333333333333343</v>
       </c>
       <c r="U35" s="1">
         <f>U49</f>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="18:21" x14ac:dyDescent="0.25">
@@ -7239,11 +7290,11 @@
       </c>
       <c r="T36" s="1">
         <f>T52</f>
-        <v>167.75200000000001</v>
+        <v>55.666666666666664</v>
       </c>
       <c r="U36" s="1">
         <f t="shared" ref="U36:U42" si="20">U50</f>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="18:21" x14ac:dyDescent="0.25">
@@ -7259,7 +7310,7 @@
       </c>
       <c r="U37" s="1">
         <f t="shared" si="20"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="38" spans="18:21" x14ac:dyDescent="0.25">
@@ -7271,11 +7322,11 @@
       </c>
       <c r="T38" s="1">
         <f>T50</f>
-        <v>111.53093333333332</v>
+        <v>67.333333333333329</v>
       </c>
       <c r="U38" s="1">
         <f t="shared" si="20"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="18:21" x14ac:dyDescent="0.25">
@@ -7287,11 +7338,11 @@
       </c>
       <c r="T39" s="1">
         <f>T53</f>
-        <v>126.7146</v>
+        <v>76.5</v>
       </c>
       <c r="U39" s="1">
         <f t="shared" si="20"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="18:21" x14ac:dyDescent="0.25">
@@ -7307,7 +7358,7 @@
       </c>
       <c r="U40" s="1">
         <f t="shared" si="20"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="18:21" x14ac:dyDescent="0.25">
@@ -7319,11 +7370,11 @@
       </c>
       <c r="T41" s="1">
         <f>T51</f>
-        <v>85.562066666666681</v>
+        <v>98.166666666666671</v>
       </c>
       <c r="U41" s="1">
         <f t="shared" si="20"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="18:21" x14ac:dyDescent="0.25">
@@ -7335,11 +7386,11 @@
       </c>
       <c r="T42" s="1">
         <f>T54</f>
-        <v>100.08873333333332</v>
+        <v>114.83333333333333</v>
       </c>
       <c r="U42" s="1">
         <f t="shared" si="20"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="43" spans="18:21" x14ac:dyDescent="0.25">
@@ -7354,8 +7405,8 @@
         <v>0</v>
       </c>
       <c r="U43" s="1">
-        <f t="shared" ref="U36:U43" si="21">U57</f>
-        <v>758.25600000000009</v>
+        <f t="shared" ref="U43" si="21">U57</f>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="18:21" x14ac:dyDescent="0.25">
@@ -7381,11 +7432,11 @@
       </c>
       <c r="T49" s="2">
         <f>T19</f>
-        <v>207.53933333333336</v>
+        <v>64.333333333333343</v>
       </c>
       <c r="U49" s="1">
         <f>U19</f>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="18:21" x14ac:dyDescent="0.25">
@@ -7394,11 +7445,11 @@
       </c>
       <c r="T50" s="2">
         <f t="shared" ref="T50:U57" si="22">T20</f>
-        <v>111.53093333333332</v>
+        <v>67.333333333333329</v>
       </c>
       <c r="U50" s="1">
         <f t="shared" si="22"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="18:21" x14ac:dyDescent="0.25">
@@ -7407,11 +7458,11 @@
       </c>
       <c r="T51" s="2">
         <f t="shared" si="22"/>
-        <v>85.562066666666681</v>
+        <v>98.166666666666671</v>
       </c>
       <c r="U51" s="1">
         <f t="shared" si="22"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="18:21" x14ac:dyDescent="0.25">
@@ -7423,11 +7474,11 @@
       </c>
       <c r="T52" s="2">
         <f t="shared" si="22"/>
-        <v>167.75200000000001</v>
+        <v>55.666666666666664</v>
       </c>
       <c r="U52" s="1">
         <f t="shared" si="22"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="18:21" x14ac:dyDescent="0.25">
@@ -7436,11 +7487,11 @@
       </c>
       <c r="T53" s="2">
         <f t="shared" si="22"/>
-        <v>126.7146</v>
+        <v>76.5</v>
       </c>
       <c r="U53" s="1">
         <f t="shared" si="22"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="18:21" x14ac:dyDescent="0.25">
@@ -7449,11 +7500,11 @@
       </c>
       <c r="T54" s="2">
         <f t="shared" si="22"/>
-        <v>100.08873333333332</v>
+        <v>114.83333333333333</v>
       </c>
       <c r="U54" s="1">
         <f t="shared" si="22"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="18:21" x14ac:dyDescent="0.25">
@@ -7469,7 +7520,7 @@
       </c>
       <c r="U55" s="1">
         <f t="shared" si="22"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="56" spans="18:21" x14ac:dyDescent="0.25">
@@ -7482,7 +7533,7 @@
       </c>
       <c r="U56" s="1">
         <f t="shared" si="22"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="18:21" x14ac:dyDescent="0.25">
@@ -7495,7 +7546,7 @@
       </c>
       <c r="U57" s="1">
         <f t="shared" si="22"/>
-        <v>758.25600000000009</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>